<commit_message>
Taller 9 casi acabado
</commit_message>
<xml_diff>
--- a/Tarea 9/Valores.xlsx
+++ b/Tarea 9/Valores.xlsx
@@ -7,7 +7,7 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="spline_coeff" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Punto 4" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -374,7 +374,17 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>y_new</t>
+          <t>Polinomial</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Lagrange</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Numpy</t>
         </is>
       </c>
     </row>
@@ -386,7 +396,13 @@
         <v>78.12</v>
       </c>
       <c r="C2" t="n">
-        <v>54.78297746765791</v>
+        <v>777.2104157209396</v>
+      </c>
+      <c r="D2" t="n">
+        <v>486226.493442297</v>
+      </c>
+      <c r="E2" t="n">
+        <v>33.84980254112725</v>
       </c>
     </row>
     <row r="3">
@@ -397,7 +413,13 @@
         <v>0.98</v>
       </c>
       <c r="C3" t="n">
-        <v>94.30652372549521</v>
+        <v>5140370.536733359</v>
+      </c>
+      <c r="D3" t="n">
+        <v>85222608.6949904</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-99.06767477112044</v>
       </c>
     </row>
     <row r="4">
@@ -408,7 +430,13 @@
         <v>67.59</v>
       </c>
       <c r="C4" t="n">
-        <v>11.79842946501877</v>
+        <v>385.5502156019211</v>
+      </c>
+      <c r="D4" t="n">
+        <v>61899.97217154503</v>
+      </c>
+      <c r="E4" t="n">
+        <v>18.19447764223423</v>
       </c>
     </row>
     <row r="5">
@@ -419,7 +447,13 @@
         <v>8.69</v>
       </c>
       <c r="C5" t="n">
-        <v>190.8282765730777</v>
+        <v>-667668.143111825</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-8935969.021080256</v>
+      </c>
+      <c r="E5" t="n">
+        <v>230.5733589715774</v>
       </c>
     </row>
     <row r="6">
@@ -430,7 +464,13 @@
         <v>55.69</v>
       </c>
       <c r="C6" t="n">
-        <v>63.65870413476917</v>
+        <v>25.73574340343475</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2858.679813146591</v>
+      </c>
+      <c r="E6" t="n">
+        <v>47.97988458354939</v>
       </c>
     </row>
     <row r="7">
@@ -441,7 +481,13 @@
         <v>48.12</v>
       </c>
       <c r="C7" t="n">
-        <v>29.617497517897</v>
+        <v>34.86005675792694</v>
+      </c>
+      <c r="D7" t="n">
+        <v>89.99121451377869</v>
+      </c>
+      <c r="E7" t="n">
+        <v>20.46013477993529</v>
       </c>
     </row>
     <row r="8">
@@ -452,7 +498,13 @@
         <v>13.24</v>
       </c>
       <c r="C8" t="n">
-        <v>-124.8260468530396</v>
+        <v>14697.83473551273</v>
+      </c>
+      <c r="D8" t="n">
+        <v>171548.7018392086</v>
+      </c>
+      <c r="E8" t="n">
+        <v>18.88264201456604</v>
       </c>
     </row>
     <row r="9">
@@ -463,7 +515,13 @@
         <v>97.56</v>
       </c>
       <c r="C9" t="n">
-        <v>88.34638231399784</v>
+        <v>8496603.760908961</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-6111427.54250741</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-4443.226321290259</v>
       </c>
     </row>
     <row r="10">
@@ -474,7 +532,13 @@
         <v>25.69</v>
       </c>
       <c r="C10" t="n">
-        <v>93.37582308647865</v>
+        <v>556.9600409269333</v>
+      </c>
+      <c r="D10" t="n">
+        <v>3567.400134801865</v>
+      </c>
+      <c r="E10" t="n">
+        <v>91.961355387818</v>
       </c>
     </row>
     <row r="11">
@@ -485,7 +549,13 @@
         <v>1.26</v>
       </c>
       <c r="C11" t="n">
-        <v>93.16047558172527</v>
+        <v>15335179.95163293</v>
+      </c>
+      <c r="D11" t="n">
+        <v>252334614.566509</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-511.2120051503416</v>
       </c>
     </row>
   </sheetData>

</xml_diff>